<commit_message>
Mini Project 1 Completed
</commit_message>
<xml_diff>
--- a/src/test/resources/data/test_datas.xlsx
+++ b/src/test/resources/data/test_datas.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20417"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:801_{9AF8810E-AF1F-416B-B025-B90A9C4D0DE1}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:801_{486F1BAF-20C5-4827-9E23-F25E733A89A4}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="17376" windowHeight="4008" activeTab="1" xr2:uid="{63300496-94F5-40F4-BDDF-0585B409FD04}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="17376" windowHeight="7608" activeTab="1" xr2:uid="{63300496-94F5-40F4-BDDF-0585B409FD04}"/>
   </bookViews>
   <sheets>
     <sheet name="Login" sheetId="2" r:id="rId1"/>
@@ -13,7 +13,7 @@
     <sheet name="AddContact" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="0"/>
-  <oleSize ref="A1:F24"/>
+  <oleSize ref="A1:F9"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -202,10 +202,10 @@
     <t>Cube</t>
   </si>
   <si>
-    <t>hatebrotest@gmail.com</t>
-  </si>
-  <si>
-    <t>Hate</t>
+    <t>Hope</t>
+  </si>
+  <si>
+    <t>HopenNopeh@gmail.com</t>
   </si>
 </sst>
 </file>
@@ -702,13 +702,13 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>4</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>22</v>
@@ -727,7 +727,7 @@
       <c r="B3" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="1" t="s">
+      <c r="C3" s="3" t="s">
         <v>21</v>
       </c>
       <c r="D3" s="1" t="s">

</xml_diff>

<commit_message>
Mini Project 1 Completed Successfully
</commit_message>
<xml_diff>
--- a/src/test/resources/data/test_datas.xlsx
+++ b/src/test/resources/data/test_datas.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20417"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:801_{486F1BAF-20C5-4827-9E23-F25E733A89A4}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:801_{4424B634-4278-4395-9B4E-5574F52DBD23}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="17376" windowHeight="7608" activeTab="1" xr2:uid="{63300496-94F5-40F4-BDDF-0585B409FD04}"/>
   </bookViews>
@@ -13,7 +13,7 @@
     <sheet name="AddContact" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="0"/>
-  <oleSize ref="A1:F9"/>
+  <oleSize ref="A1:F24"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -205,7 +205,7 @@
     <t>Hope</t>
   </si>
   <si>
-    <t>HopenNopeh@gmail.com</t>
+    <t>HopenNh@gmail.com</t>
   </si>
 </sst>
 </file>

</xml_diff>